<commit_message>
Deploying to gh-pages from @ Healthedata1/USCDI5-Sandbox@c6272baa640535dea50ed044fe8d4297e4550178 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-us-core-observation-adi-documentation.xlsx
+++ b/StructureDefinition-us-core-observation-adi-documentation.xlsx
@@ -817,10 +817,10 @@
     <t>Clinically relevant time/time-period for observation</t>
   </si>
   <si>
-    <t>The time or time-period the observed value is asserted as being true. For biological subjects - e.g., human patients - this is usually called the "physiologically relevant time".</t>
-  </si>
-  <si>
-    <t>At least a date should be present unless this observation is a historical report.</t>
+    <t>The time or time-period the observed value is asserted as being true. For biological subjects - e.g. human patients - this is usually called the "physiologically relevant time". This is usually either the time of the procedure or of specimen collection, but very often the source of the date/time is not known, only the date/time itself.</t>
+  </si>
+  <si>
+    <t>At least a date should be present unless this observation is a historical report.  For recording imprecise or "fuzzy" times (For example, a blood glucose measurement taken "after breakfast") use the [Timing](http://hl7.org/fhir/R4/datatypes.html#timing) datatype which allow the measurement to be tied to regular life events.</t>
   </si>
   <si>
     <t>Knowing when an observation was deemed true is important to its relevance as well as determining trends.</t>
@@ -845,7 +845,7 @@
 </t>
   </si>
   <si>
-    <t>Date/Time this version was made available</t>
+    <t>Date/Time this reviewed and verified observation was made available</t>
   </si>
   <si>
     <t>The date and time this version of the observation was made available to providers, typically after the results have been reviewed and verified.</t>
@@ -866,11 +866,11 @@
     <t>Observation.performer</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Practitioner|PractitionerRole|Organization|CareTeam|Patient|RelatedPerson)
+    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitioner|http://hl7.org/fhir/us/core/StructureDefinition/us-core-organization|http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient|PractitionerRole|http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam|http://hl7.org/fhir/us/core/StructureDefinition/us-core-relatedperson)
 </t>
   </si>
   <si>
-    <t>Who is responsible for the observation</t>
+    <t>Who reviewed and verified the observation</t>
   </si>
   <si>
     <t>Who was responsible for asserting the observed value as "true".</t>
@@ -909,10 +909,10 @@
     <t>extensible</t>
   </si>
   <si>
-    <t>ADI documentation types</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/ValueSet/us-core-adi-finding</t>
+    <t>Advance Healthcare Directive Categories Grouper</t>
+  </si>
+  <si>
+    <t>http://cts.nlm.nih.gov/fhir/ValueSet/2.16.840.1.113762.1.4.1115.25</t>
   </si>
   <si>
     <t xml:space="preserve">obs-7
@@ -1806,7 +1806,7 @@
     <col min="8" max="8" width="16.27734375" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="13.26171875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="111.11328125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="255.0" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1821,7 +1821,7 @@
     <col min="23" max="23" width="19.03515625" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="18.859375" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="63.70703125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="50.8203125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="63.01953125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="20.59375" customWidth="true" bestFit="true"/>
@@ -4278,7 +4278,7 @@
         <v>94</v>
       </c>
       <c r="H21" t="s" s="2">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="I21" t="s" s="2">
         <v>84</v>
@@ -4400,7 +4400,7 @@
         <v>94</v>
       </c>
       <c r="H22" t="s" s="2">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="I22" t="s" s="2">
         <v>84</v>
@@ -4520,7 +4520,7 @@
         <v>83</v>
       </c>
       <c r="H23" t="s" s="2">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="I23" t="s" s="2">
         <v>84</v>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ Healthedata1/USCDI5-Sandbox@0b420f4d5cbdf153dd1b09c448c2a9bac880a179 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-us-core-observation-adi-documentation.xlsx
+++ b/StructureDefinition-us-core-observation-adi-documentation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2039" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2039" uniqueCount="458">
   <si>
     <t>Property</t>
   </si>
@@ -63,7 +63,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-05-30</t>
+    <t>2024-09-13</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -90,7 +90,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>The US Core Observation ADI Documentation Profile inherits from the FHIR [Observation](https://hl7.org/fhir/R4/observation.html) resource; refer to it for scope and usage definitions. This profile is used to indicate if additional advance directive documents, such as physician order for life sustaining treatment (MOLST or POLST) or Do Not Resuscitate Order (DNR) exist and a reference to the document. The observation is not intended to communicate the actual contents of those additional documents, if they exist, but are intended to represent that the documents exist so that further investigation can be undertaken to locate them or learn more about them. This profile sets minimum expectations for the Observation resource to record, search, and fetch findings about ADI Documentation. It specifies which core elements, extensions,  vocabularies, and value sets **SHALL** be present in the resource and constrains how the elements are used. Providing the floor for standards development for specific use cases promotes interoperability and adoption.</t>
+    <t>The US Core Observation ADI Documentation Profile inherits from the FHIR [Observation](https://hl7.org/fhir/R4/observation.html) resource; refer to it for scope and usage definitions. This profile and the [US Core Observation ADI Presence Profile] together meet the requirements of the U.S. Core Data for Interoperability (USCDI) *Advance Directive Observation* Data Element. It is used to communicate the types of advance directive documents for a patient, the document location, and other properties. Examples of advance healthcare directive documents include physician order for life sustaining treatment (POLST), do not resuscitate order (DNR), and medical power of attorney. To communicates whether any advance directive documents exist for a patient, see the [US Core Observation ADI Presence Profile]. This profile sets minimum expectations for the Observation resource to record, search, and fetch findings about advance directive documents. It specifies which core elements, extensions,  vocabularies, and value sets **SHALL** be present in the resource and constrains how the elements are used. Providing the floor for standards development for specific use cases promotes interoperability and adoption.</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -683,21 +683,13 @@
     <t>Knowing what kind of observation is being made is essential to understanding the observation.</t>
   </si>
   <si>
-    <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
-  &lt;coding&gt;
-    &lt;system value="http://loinc.org"/&gt;
-    &lt;code value="42348-3"/&gt;
-  &lt;/coding&gt;
-&lt;/valueCodeableConcept&gt;</t>
-  </si>
-  <si>
-    <t>example</t>
-  </si>
-  <si>
-    <t>Codes identifying names of simple observations.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/observation-codes</t>
+    <t>extensible</t>
+  </si>
+  <si>
+    <t>Category of advance directive</t>
+  </si>
+  <si>
+    <t>http://cts.nlm.nih.gov/fhir/ValueSet/2.16.840.1.113762.1.4.1115.25</t>
   </si>
   <si>
     <t>Event.code</t>
@@ -906,13 +898,10 @@
     <t>An observation exists to have a value, though it might not if it is in error, or if it represents a group of observations.</t>
   </si>
   <si>
-    <t>extensible</t>
-  </si>
-  <si>
-    <t>Advance Healthcare Directive Categories Grouper</t>
-  </si>
-  <si>
-    <t>http://cts.nlm.nih.gov/fhir/ValueSet/2.16.840.1.113762.1.4.1115.25</t>
+    <t>Type of advance directive document</t>
+  </si>
+  <si>
+    <t>http://cts.nlm.nih.gov/fhir/ValueSet/2.16.840.1.113762.1.4.1099.57</t>
   </si>
   <si>
     <t xml:space="preserve">obs-7
@@ -1033,6 +1022,9 @@
   <si>
     <t>Only used if not implicit in code found in Observation.code.  In many systems, this may be represented as a related observation instead of an inline component.   
 If the use case requires BodySite to be handled as a separate resource (e.g. to identify and track separately) then use the standard extension[ bodySite](http://hl7.org/fhir/R4/extension-bodysite.html).</t>
+  </si>
+  <si>
+    <t>example</t>
   </si>
   <si>
     <t>Codes describing anatomical locations. May include laterality.</t>
@@ -1411,6 +1403,12 @@
   </si>
   <si>
     <t>*All* code-value and  component.code-component.value pairs need to be taken into account to correctly understand the meaning of the observation.</t>
+  </si>
+  <si>
+    <t>Codes identifying names of simple observations.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/observation-codes</t>
   </si>
   <si>
     <t>&lt; 363787002 |Observable entity| OR @@ -3823,28 +3821,28 @@
         <v>84</v>
       </c>
       <c r="S17" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="T17" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="U17" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="V17" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="W17" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="X17" t="s" s="2">
         <v>212</v>
       </c>
-      <c r="T17" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="U17" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="V17" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="W17" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="X17" t="s" s="2">
+      <c r="Y17" t="s" s="2">
         <v>213</v>
       </c>
-      <c r="Y17" t="s" s="2">
+      <c r="Z17" t="s" s="2">
         <v>214</v>
-      </c>
-      <c r="Z17" t="s" s="2">
-        <v>215</v>
       </c>
       <c r="AA17" t="s" s="2">
         <v>84</v>
@@ -3877,30 +3875,30 @@
         <v>106</v>
       </c>
       <c r="AK17" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="AL17" t="s" s="2">
         <v>216</v>
       </c>
-      <c r="AL17" t="s" s="2">
+      <c r="AM17" t="s" s="2">
         <v>217</v>
       </c>
-      <c r="AM17" t="s" s="2">
+      <c r="AN17" t="s" s="2">
         <v>218</v>
       </c>
-      <c r="AN17" t="s" s="2">
+      <c r="AO17" t="s" s="2">
         <v>219</v>
       </c>
-      <c r="AO17" t="s" s="2">
+      <c r="AP17" t="s" s="2">
         <v>220</v>
-      </c>
-      <c r="AP17" t="s" s="2">
-        <v>221</v>
       </c>
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
@@ -3923,19 +3921,19 @@
         <v>95</v>
       </c>
       <c r="K18" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="L18" t="s" s="2">
         <v>223</v>
       </c>
-      <c r="L18" t="s" s="2">
+      <c r="M18" t="s" s="2">
         <v>224</v>
       </c>
-      <c r="M18" t="s" s="2">
+      <c r="N18" t="s" s="2">
         <v>225</v>
       </c>
-      <c r="N18" t="s" s="2">
+      <c r="O18" t="s" s="2">
         <v>226</v>
-      </c>
-      <c r="O18" t="s" s="2">
-        <v>227</v>
       </c>
       <c r="P18" t="s" s="2">
         <v>84</v>
@@ -3984,7 +3982,7 @@
         <v>84</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>82</v>
@@ -3999,19 +3997,19 @@
         <v>106</v>
       </c>
       <c r="AK18" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="AL18" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AM18" t="s" s="2">
         <v>228</v>
       </c>
-      <c r="AL18" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AM18" t="s" s="2">
+      <c r="AN18" t="s" s="2">
         <v>229</v>
       </c>
-      <c r="AN18" t="s" s="2">
+      <c r="AO18" t="s" s="2">
         <v>230</v>
-      </c>
-      <c r="AO18" t="s" s="2">
-        <v>231</v>
       </c>
       <c r="AP18" t="s" s="2">
         <v>84</v>
@@ -4019,10 +4017,10 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
@@ -4045,16 +4043,16 @@
         <v>95</v>
       </c>
       <c r="K19" t="s" s="2">
+        <v>232</v>
+      </c>
+      <c r="L19" t="s" s="2">
         <v>233</v>
       </c>
-      <c r="L19" t="s" s="2">
+      <c r="M19" t="s" s="2">
         <v>234</v>
       </c>
-      <c r="M19" t="s" s="2">
+      <c r="N19" t="s" s="2">
         <v>235</v>
-      </c>
-      <c r="N19" t="s" s="2">
-        <v>236</v>
       </c>
       <c r="O19" s="2"/>
       <c r="P19" t="s" s="2">
@@ -4104,7 +4102,7 @@
         <v>84</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>82</v>
@@ -4125,13 +4123,13 @@
         <v>84</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AN19" t="s" s="2">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AO19" t="s" s="2">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AP19" t="s" s="2">
         <v>84</v>
@@ -4139,14 +4137,14 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" t="s" s="2">
@@ -4165,19 +4163,19 @@
         <v>95</v>
       </c>
       <c r="K20" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="L20" t="s" s="2">
         <v>240</v>
       </c>
-      <c r="L20" t="s" s="2">
+      <c r="M20" t="s" s="2">
         <v>241</v>
       </c>
-      <c r="M20" t="s" s="2">
+      <c r="N20" t="s" s="2">
         <v>242</v>
       </c>
-      <c r="N20" t="s" s="2">
+      <c r="O20" t="s" s="2">
         <v>243</v>
-      </c>
-      <c r="O20" t="s" s="2">
-        <v>244</v>
       </c>
       <c r="P20" t="s" s="2">
         <v>84</v>
@@ -4226,7 +4224,7 @@
         <v>84</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>82</v>
@@ -4241,19 +4239,19 @@
         <v>106</v>
       </c>
       <c r="AK20" t="s" s="2">
+        <v>244</v>
+      </c>
+      <c r="AL20" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AM20" t="s" s="2">
         <v>245</v>
       </c>
-      <c r="AL20" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AM20" t="s" s="2">
+      <c r="AN20" t="s" s="2">
         <v>246</v>
       </c>
-      <c r="AN20" t="s" s="2">
+      <c r="AO20" t="s" s="2">
         <v>247</v>
-      </c>
-      <c r="AO20" t="s" s="2">
-        <v>248</v>
       </c>
       <c r="AP20" t="s" s="2">
         <v>84</v>
@@ -4261,14 +4259,14 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" t="s" s="2">
@@ -4287,19 +4285,19 @@
         <v>95</v>
       </c>
       <c r="K21" t="s" s="2">
+        <v>250</v>
+      </c>
+      <c r="L21" t="s" s="2">
         <v>251</v>
       </c>
-      <c r="L21" t="s" s="2">
+      <c r="M21" t="s" s="2">
         <v>252</v>
       </c>
-      <c r="M21" t="s" s="2">
+      <c r="N21" t="s" s="2">
         <v>253</v>
       </c>
-      <c r="N21" t="s" s="2">
+      <c r="O21" t="s" s="2">
         <v>254</v>
-      </c>
-      <c r="O21" t="s" s="2">
-        <v>255</v>
       </c>
       <c r="P21" t="s" s="2">
         <v>84</v>
@@ -4348,7 +4346,7 @@
         <v>84</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>82</v>
@@ -4363,19 +4361,19 @@
         <v>106</v>
       </c>
       <c r="AK21" t="s" s="2">
+        <v>255</v>
+      </c>
+      <c r="AL21" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AM21" t="s" s="2">
         <v>256</v>
       </c>
-      <c r="AL21" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AM21" t="s" s="2">
+      <c r="AN21" t="s" s="2">
         <v>257</v>
       </c>
-      <c r="AN21" t="s" s="2">
+      <c r="AO21" t="s" s="2">
         <v>258</v>
-      </c>
-      <c r="AO21" t="s" s="2">
-        <v>259</v>
       </c>
       <c r="AP21" t="s" s="2">
         <v>84</v>
@@ -4383,10 +4381,10 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -4409,16 +4407,16 @@
         <v>95</v>
       </c>
       <c r="K22" t="s" s="2">
+        <v>260</v>
+      </c>
+      <c r="L22" t="s" s="2">
         <v>261</v>
       </c>
-      <c r="L22" t="s" s="2">
+      <c r="M22" t="s" s="2">
         <v>262</v>
       </c>
-      <c r="M22" t="s" s="2">
+      <c r="N22" t="s" s="2">
         <v>263</v>
-      </c>
-      <c r="N22" t="s" s="2">
-        <v>264</v>
       </c>
       <c r="O22" s="2"/>
       <c r="P22" t="s" s="2">
@@ -4468,7 +4466,7 @@
         <v>84</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>82</v>
@@ -4489,13 +4487,13 @@
         <v>84</v>
       </c>
       <c r="AM22" t="s" s="2">
+        <v>264</v>
+      </c>
+      <c r="AN22" t="s" s="2">
         <v>265</v>
       </c>
-      <c r="AN22" t="s" s="2">
+      <c r="AO22" t="s" s="2">
         <v>266</v>
-      </c>
-      <c r="AO22" t="s" s="2">
-        <v>267</v>
       </c>
       <c r="AP22" t="s" s="2">
         <v>84</v>
@@ -4503,10 +4501,10 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
@@ -4529,17 +4527,17 @@
         <v>95</v>
       </c>
       <c r="K23" t="s" s="2">
+        <v>268</v>
+      </c>
+      <c r="L23" t="s" s="2">
         <v>269</v>
       </c>
-      <c r="L23" t="s" s="2">
+      <c r="M23" t="s" s="2">
         <v>270</v>
-      </c>
-      <c r="M23" t="s" s="2">
-        <v>271</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="P23" t="s" s="2">
         <v>84</v>
@@ -4588,7 +4586,7 @@
         <v>84</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>82</v>
@@ -4603,19 +4601,19 @@
         <v>106</v>
       </c>
       <c r="AK23" t="s" s="2">
+        <v>272</v>
+      </c>
+      <c r="AL23" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AM23" t="s" s="2">
         <v>273</v>
       </c>
-      <c r="AL23" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AM23" t="s" s="2">
+      <c r="AN23" t="s" s="2">
         <v>274</v>
       </c>
-      <c r="AN23" t="s" s="2">
+      <c r="AO23" t="s" s="2">
         <v>275</v>
-      </c>
-      <c r="AO23" t="s" s="2">
-        <v>276</v>
       </c>
       <c r="AP23" t="s" s="2">
         <v>84</v>
@@ -4623,10 +4621,10 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
@@ -4652,16 +4650,16 @@
         <v>192</v>
       </c>
       <c r="L24" t="s" s="2">
+        <v>277</v>
+      </c>
+      <c r="M24" t="s" s="2">
         <v>278</v>
       </c>
-      <c r="M24" t="s" s="2">
+      <c r="N24" t="s" s="2">
         <v>279</v>
       </c>
-      <c r="N24" t="s" s="2">
+      <c r="O24" t="s" s="2">
         <v>280</v>
-      </c>
-      <c r="O24" t="s" s="2">
-        <v>281</v>
       </c>
       <c r="P24" t="s" s="2">
         <v>84</v>
@@ -4686,14 +4684,14 @@
         <v>84</v>
       </c>
       <c r="X24" t="s" s="2">
+        <v>212</v>
+      </c>
+      <c r="Y24" t="s" s="2">
+        <v>281</v>
+      </c>
+      <c r="Z24" t="s" s="2">
         <v>282</v>
       </c>
-      <c r="Y24" t="s" s="2">
-        <v>283</v>
-      </c>
-      <c r="Z24" t="s" s="2">
-        <v>284</v>
-      </c>
       <c r="AA24" t="s" s="2">
         <v>84</v>
       </c>
@@ -4710,7 +4708,7 @@
         <v>84</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>82</v>
@@ -4719,7 +4717,7 @@
         <v>94</v>
       </c>
       <c r="AI24" t="s" s="2">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="AJ24" t="s" s="2">
         <v>106</v>
@@ -4728,27 +4726,27 @@
         <v>84</v>
       </c>
       <c r="AL24" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="AM24" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="AN24" t="s" s="2">
         <v>286</v>
       </c>
-      <c r="AM24" t="s" s="2">
+      <c r="AO24" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AP24" t="s" s="2">
         <v>287</v>
-      </c>
-      <c r="AN24" t="s" s="2">
-        <v>288</v>
-      </c>
-      <c r="AO24" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AP24" t="s" s="2">
-        <v>289</v>
       </c>
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
@@ -4774,16 +4772,16 @@
         <v>192</v>
       </c>
       <c r="L25" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="M25" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="N25" t="s" s="2">
         <v>291</v>
       </c>
-      <c r="M25" t="s" s="2">
+      <c r="O25" t="s" s="2">
         <v>292</v>
-      </c>
-      <c r="N25" t="s" s="2">
-        <v>293</v>
-      </c>
-      <c r="O25" t="s" s="2">
-        <v>294</v>
       </c>
       <c r="P25" t="s" s="2">
         <v>84</v>
@@ -4808,13 +4806,13 @@
         <v>84</v>
       </c>
       <c r="X25" t="s" s="2">
-        <v>282</v>
+        <v>212</v>
       </c>
       <c r="Y25" t="s" s="2">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="Z25" t="s" s="2">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="AA25" t="s" s="2">
         <v>84</v>
@@ -4832,7 +4830,7 @@
         <v>84</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>82</v>
@@ -4841,7 +4839,7 @@
         <v>94</v>
       </c>
       <c r="AI25" t="s" s="2">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AJ25" t="s" s="2">
         <v>106</v>
@@ -4856,7 +4854,7 @@
         <v>137</v>
       </c>
       <c r="AN25" t="s" s="2">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AO25" t="s" s="2">
         <v>84</v>
@@ -4867,14 +4865,14 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" t="s" s="2">
@@ -4896,16 +4894,16 @@
         <v>192</v>
       </c>
       <c r="L26" t="s" s="2">
+        <v>299</v>
+      </c>
+      <c r="M26" t="s" s="2">
+        <v>300</v>
+      </c>
+      <c r="N26" t="s" s="2">
         <v>301</v>
       </c>
-      <c r="M26" t="s" s="2">
+      <c r="O26" t="s" s="2">
         <v>302</v>
-      </c>
-      <c r="N26" t="s" s="2">
-        <v>303</v>
-      </c>
-      <c r="O26" t="s" s="2">
-        <v>304</v>
       </c>
       <c r="P26" t="s" s="2">
         <v>84</v>
@@ -4930,13 +4928,13 @@
         <v>84</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>282</v>
+        <v>212</v>
       </c>
       <c r="Y26" t="s" s="2">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="Z26" t="s" s="2">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="AA26" t="s" s="2">
         <v>84</v>
@@ -4954,7 +4952,7 @@
         <v>84</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>82</v>
@@ -4972,27 +4970,27 @@
         <v>84</v>
       </c>
       <c r="AL26" t="s" s="2">
+        <v>305</v>
+      </c>
+      <c r="AM26" t="s" s="2">
+        <v>306</v>
+      </c>
+      <c r="AN26" t="s" s="2">
         <v>307</v>
       </c>
-      <c r="AM26" t="s" s="2">
+      <c r="AO26" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AP26" t="s" s="2">
         <v>308</v>
-      </c>
-      <c r="AN26" t="s" s="2">
-        <v>309</v>
-      </c>
-      <c r="AO26" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AP26" t="s" s="2">
-        <v>310</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -5015,19 +5013,19 @@
         <v>84</v>
       </c>
       <c r="K27" t="s" s="2">
+        <v>310</v>
+      </c>
+      <c r="L27" t="s" s="2">
+        <v>311</v>
+      </c>
+      <c r="M27" t="s" s="2">
         <v>312</v>
       </c>
-      <c r="L27" t="s" s="2">
+      <c r="N27" t="s" s="2">
         <v>313</v>
       </c>
-      <c r="M27" t="s" s="2">
+      <c r="O27" t="s" s="2">
         <v>314</v>
-      </c>
-      <c r="N27" t="s" s="2">
-        <v>315</v>
-      </c>
-      <c r="O27" t="s" s="2">
-        <v>316</v>
       </c>
       <c r="P27" t="s" s="2">
         <v>84</v>
@@ -5076,7 +5074,7 @@
         <v>84</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>82</v>
@@ -5097,10 +5095,10 @@
         <v>84</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AN27" t="s" s="2">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AO27" t="s" s="2">
         <v>84</v>
@@ -5111,10 +5109,10 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
@@ -5140,13 +5138,13 @@
         <v>192</v>
       </c>
       <c r="L28" t="s" s="2">
+        <v>318</v>
+      </c>
+      <c r="M28" t="s" s="2">
+        <v>319</v>
+      </c>
+      <c r="N28" t="s" s="2">
         <v>320</v>
-      </c>
-      <c r="M28" t="s" s="2">
-        <v>321</v>
-      </c>
-      <c r="N28" t="s" s="2">
-        <v>322</v>
       </c>
       <c r="O28" s="2"/>
       <c r="P28" t="s" s="2">
@@ -5172,14 +5170,14 @@
         <v>84</v>
       </c>
       <c r="X28" t="s" s="2">
-        <v>213</v>
+        <v>321</v>
       </c>
       <c r="Y28" t="s" s="2">
+        <v>322</v>
+      </c>
+      <c r="Z28" t="s" s="2">
         <v>323</v>
       </c>
-      <c r="Z28" t="s" s="2">
-        <v>324</v>
-      </c>
       <c r="AA28" t="s" s="2">
         <v>84</v>
       </c>
@@ -5196,7 +5194,7 @@
         <v>84</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>82</v>
@@ -5214,27 +5212,27 @@
         <v>84</v>
       </c>
       <c r="AL28" t="s" s="2">
+        <v>324</v>
+      </c>
+      <c r="AM28" t="s" s="2">
         <v>325</v>
       </c>
-      <c r="AM28" t="s" s="2">
+      <c r="AN28" t="s" s="2">
         <v>326</v>
       </c>
-      <c r="AN28" t="s" s="2">
+      <c r="AO28" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AP28" t="s" s="2">
         <v>327</v>
-      </c>
-      <c r="AO28" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AP28" t="s" s="2">
-        <v>328</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -5260,16 +5258,16 @@
         <v>192</v>
       </c>
       <c r="L29" t="s" s="2">
+        <v>329</v>
+      </c>
+      <c r="M29" t="s" s="2">
         <v>330</v>
       </c>
-      <c r="M29" t="s" s="2">
+      <c r="N29" t="s" s="2">
         <v>331</v>
       </c>
-      <c r="N29" t="s" s="2">
+      <c r="O29" t="s" s="2">
         <v>332</v>
-      </c>
-      <c r="O29" t="s" s="2">
-        <v>333</v>
       </c>
       <c r="P29" t="s" s="2">
         <v>84</v>
@@ -5294,14 +5292,14 @@
         <v>84</v>
       </c>
       <c r="X29" t="s" s="2">
-        <v>213</v>
+        <v>321</v>
       </c>
       <c r="Y29" t="s" s="2">
+        <v>333</v>
+      </c>
+      <c r="Z29" t="s" s="2">
         <v>334</v>
       </c>
-      <c r="Z29" t="s" s="2">
-        <v>335</v>
-      </c>
       <c r="AA29" t="s" s="2">
         <v>84</v>
       </c>
@@ -5318,7 +5316,7 @@
         <v>84</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>82</v>
@@ -5339,10 +5337,10 @@
         <v>84</v>
       </c>
       <c r="AM29" t="s" s="2">
+        <v>335</v>
+      </c>
+      <c r="AN29" t="s" s="2">
         <v>336</v>
-      </c>
-      <c r="AN29" t="s" s="2">
-        <v>337</v>
       </c>
       <c r="AO29" t="s" s="2">
         <v>84</v>
@@ -5353,10 +5351,10 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -5379,16 +5377,16 @@
         <v>84</v>
       </c>
       <c r="K30" t="s" s="2">
+        <v>338</v>
+      </c>
+      <c r="L30" t="s" s="2">
         <v>339</v>
       </c>
-      <c r="L30" t="s" s="2">
+      <c r="M30" t="s" s="2">
         <v>340</v>
       </c>
-      <c r="M30" t="s" s="2">
+      <c r="N30" t="s" s="2">
         <v>341</v>
-      </c>
-      <c r="N30" t="s" s="2">
-        <v>342</v>
       </c>
       <c r="O30" s="2"/>
       <c r="P30" t="s" s="2">
@@ -5438,7 +5436,7 @@
         <v>84</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>82</v>
@@ -5456,27 +5454,27 @@
         <v>84</v>
       </c>
       <c r="AL30" t="s" s="2">
+        <v>342</v>
+      </c>
+      <c r="AM30" t="s" s="2">
         <v>343</v>
       </c>
-      <c r="AM30" t="s" s="2">
+      <c r="AN30" t="s" s="2">
         <v>344</v>
       </c>
-      <c r="AN30" t="s" s="2">
+      <c r="AO30" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AP30" t="s" s="2">
         <v>345</v>
-      </c>
-      <c r="AO30" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AP30" t="s" s="2">
-        <v>346</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -5499,16 +5497,16 @@
         <v>84</v>
       </c>
       <c r="K31" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="L31" t="s" s="2">
         <v>348</v>
       </c>
-      <c r="L31" t="s" s="2">
+      <c r="M31" t="s" s="2">
         <v>349</v>
       </c>
-      <c r="M31" t="s" s="2">
+      <c r="N31" t="s" s="2">
         <v>350</v>
-      </c>
-      <c r="N31" t="s" s="2">
-        <v>351</v>
       </c>
       <c r="O31" s="2"/>
       <c r="P31" t="s" s="2">
@@ -5558,7 +5556,7 @@
         <v>84</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>82</v>
@@ -5576,27 +5574,27 @@
         <v>84</v>
       </c>
       <c r="AL31" t="s" s="2">
+        <v>351</v>
+      </c>
+      <c r="AM31" t="s" s="2">
         <v>352</v>
       </c>
-      <c r="AM31" t="s" s="2">
+      <c r="AN31" t="s" s="2">
         <v>353</v>
       </c>
-      <c r="AN31" t="s" s="2">
+      <c r="AO31" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AP31" t="s" s="2">
         <v>354</v>
-      </c>
-      <c r="AO31" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AP31" t="s" s="2">
-        <v>355</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -5619,19 +5617,19 @@
         <v>84</v>
       </c>
       <c r="K32" t="s" s="2">
+        <v>356</v>
+      </c>
+      <c r="L32" t="s" s="2">
         <v>357</v>
       </c>
-      <c r="L32" t="s" s="2">
+      <c r="M32" t="s" s="2">
         <v>358</v>
       </c>
-      <c r="M32" t="s" s="2">
+      <c r="N32" t="s" s="2">
         <v>359</v>
       </c>
-      <c r="N32" t="s" s="2">
+      <c r="O32" t="s" s="2">
         <v>360</v>
-      </c>
-      <c r="O32" t="s" s="2">
-        <v>361</v>
       </c>
       <c r="P32" t="s" s="2">
         <v>84</v>
@@ -5680,7 +5678,7 @@
         <v>84</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>82</v>
@@ -5692,19 +5690,19 @@
         <v>84</v>
       </c>
       <c r="AJ32" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="AK32" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AL32" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AM32" t="s" s="2">
         <v>362</v>
       </c>
-      <c r="AK32" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AL32" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AM32" t="s" s="2">
+      <c r="AN32" t="s" s="2">
         <v>363</v>
-      </c>
-      <c r="AN32" t="s" s="2">
-        <v>364</v>
       </c>
       <c r="AO32" t="s" s="2">
         <v>84</v>
@@ -5715,10 +5713,10 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5741,13 +5739,13 @@
         <v>84</v>
       </c>
       <c r="K33" t="s" s="2">
+        <v>365</v>
+      </c>
+      <c r="L33" t="s" s="2">
         <v>366</v>
       </c>
-      <c r="L33" t="s" s="2">
+      <c r="M33" t="s" s="2">
         <v>367</v>
-      </c>
-      <c r="M33" t="s" s="2">
-        <v>368</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
@@ -5798,7 +5796,7 @@
         <v>84</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>82</v>
@@ -5822,7 +5820,7 @@
         <v>84</v>
       </c>
       <c r="AN33" t="s" s="2">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="AO33" t="s" s="2">
         <v>84</v>
@@ -5833,10 +5831,10 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5865,7 +5863,7 @@
         <v>141</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="N34" t="s" s="2">
         <v>143</v>
@@ -5918,7 +5916,7 @@
         <v>84</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>82</v>
@@ -5942,7 +5940,7 @@
         <v>84</v>
       </c>
       <c r="AN34" t="s" s="2">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="AO34" t="s" s="2">
         <v>84</v>
@@ -5953,14 +5951,14 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" t="s" s="2">
@@ -5982,10 +5980,10 @@
         <v>140</v>
       </c>
       <c r="L35" t="s" s="2">
+        <v>375</v>
+      </c>
+      <c r="M35" t="s" s="2">
         <v>376</v>
-      </c>
-      <c r="M35" t="s" s="2">
-        <v>377</v>
       </c>
       <c r="N35" t="s" s="2">
         <v>143</v>
@@ -6040,7 +6038,7 @@
         <v>84</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>82</v>
@@ -6075,10 +6073,10 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -6101,13 +6099,13 @@
         <v>84</v>
       </c>
       <c r="K36" t="s" s="2">
+        <v>379</v>
+      </c>
+      <c r="L36" t="s" s="2">
         <v>380</v>
       </c>
-      <c r="L36" t="s" s="2">
+      <c r="M36" t="s" s="2">
         <v>381</v>
-      </c>
-      <c r="M36" t="s" s="2">
-        <v>382</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
@@ -6158,7 +6156,7 @@
         <v>84</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>82</v>
@@ -6167,7 +6165,7 @@
         <v>94</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="AJ36" t="s" s="2">
         <v>106</v>
@@ -6179,10 +6177,10 @@
         <v>84</v>
       </c>
       <c r="AM36" t="s" s="2">
+        <v>383</v>
+      </c>
+      <c r="AN36" t="s" s="2">
         <v>384</v>
-      </c>
-      <c r="AN36" t="s" s="2">
-        <v>385</v>
       </c>
       <c r="AO36" t="s" s="2">
         <v>84</v>
@@ -6193,10 +6191,10 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -6219,13 +6217,13 @@
         <v>84</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="L37" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="M37" t="s" s="2">
         <v>387</v>
-      </c>
-      <c r="M37" t="s" s="2">
-        <v>388</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
@@ -6276,7 +6274,7 @@
         <v>84</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>82</v>
@@ -6285,7 +6283,7 @@
         <v>94</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="AJ37" t="s" s="2">
         <v>106</v>
@@ -6297,10 +6295,10 @@
         <v>84</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AN37" t="s" s="2">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="AO37" t="s" s="2">
         <v>84</v>
@@ -6311,10 +6309,10 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -6340,16 +6338,16 @@
         <v>192</v>
       </c>
       <c r="L38" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="M38" t="s" s="2">
         <v>391</v>
       </c>
-      <c r="M38" t="s" s="2">
+      <c r="N38" t="s" s="2">
         <v>392</v>
       </c>
-      <c r="N38" t="s" s="2">
+      <c r="O38" t="s" s="2">
         <v>393</v>
-      </c>
-      <c r="O38" t="s" s="2">
-        <v>394</v>
       </c>
       <c r="P38" t="s" s="2">
         <v>84</v>
@@ -6377,11 +6375,11 @@
         <v>118</v>
       </c>
       <c r="Y38" t="s" s="2">
+        <v>394</v>
+      </c>
+      <c r="Z38" t="s" s="2">
         <v>395</v>
       </c>
-      <c r="Z38" t="s" s="2">
-        <v>396</v>
-      </c>
       <c r="AA38" t="s" s="2">
         <v>84</v>
       </c>
@@ -6398,7 +6396,7 @@
         <v>84</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>82</v>
@@ -6416,13 +6414,13 @@
         <v>84</v>
       </c>
       <c r="AL38" t="s" s="2">
+        <v>396</v>
+      </c>
+      <c r="AM38" t="s" s="2">
         <v>397</v>
       </c>
-      <c r="AM38" t="s" s="2">
-        <v>398</v>
-      </c>
       <c r="AN38" t="s" s="2">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="AO38" t="s" s="2">
         <v>84</v>
@@ -6433,10 +6431,10 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -6462,16 +6460,16 @@
         <v>192</v>
       </c>
       <c r="L39" t="s" s="2">
+        <v>399</v>
+      </c>
+      <c r="M39" t="s" s="2">
         <v>400</v>
       </c>
-      <c r="M39" t="s" s="2">
+      <c r="N39" t="s" s="2">
         <v>401</v>
       </c>
-      <c r="N39" t="s" s="2">
+      <c r="O39" t="s" s="2">
         <v>402</v>
-      </c>
-      <c r="O39" t="s" s="2">
-        <v>403</v>
       </c>
       <c r="P39" t="s" s="2">
         <v>84</v>
@@ -6496,14 +6494,14 @@
         <v>84</v>
       </c>
       <c r="X39" t="s" s="2">
-        <v>213</v>
+        <v>321</v>
       </c>
       <c r="Y39" t="s" s="2">
+        <v>403</v>
+      </c>
+      <c r="Z39" t="s" s="2">
         <v>404</v>
       </c>
-      <c r="Z39" t="s" s="2">
-        <v>405</v>
-      </c>
       <c r="AA39" t="s" s="2">
         <v>84</v>
       </c>
@@ -6520,7 +6518,7 @@
         <v>84</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>82</v>
@@ -6538,13 +6536,13 @@
         <v>84</v>
       </c>
       <c r="AL39" t="s" s="2">
+        <v>396</v>
+      </c>
+      <c r="AM39" t="s" s="2">
         <v>397</v>
       </c>
-      <c r="AM39" t="s" s="2">
-        <v>398</v>
-      </c>
       <c r="AN39" t="s" s="2">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="AO39" t="s" s="2">
         <v>84</v>
@@ -6555,10 +6553,10 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -6581,17 +6579,17 @@
         <v>84</v>
       </c>
       <c r="K40" t="s" s="2">
+        <v>406</v>
+      </c>
+      <c r="L40" t="s" s="2">
         <v>407</v>
       </c>
-      <c r="L40" t="s" s="2">
+      <c r="M40" t="s" s="2">
         <v>408</v>
-      </c>
-      <c r="M40" t="s" s="2">
-        <v>409</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" t="s" s="2">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="P40" t="s" s="2">
         <v>84</v>
@@ -6640,7 +6638,7 @@
         <v>84</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>82</v>
@@ -6664,7 +6662,7 @@
         <v>84</v>
       </c>
       <c r="AN40" t="s" s="2">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="AO40" t="s" s="2">
         <v>84</v>
@@ -6675,10 +6673,10 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -6701,13 +6699,13 @@
         <v>84</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="L41" t="s" s="2">
+        <v>412</v>
+      </c>
+      <c r="M41" t="s" s="2">
         <v>413</v>
-      </c>
-      <c r="M41" t="s" s="2">
-        <v>414</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
@@ -6758,7 +6756,7 @@
         <v>84</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>82</v>
@@ -6779,10 +6777,10 @@
         <v>84</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AN41" t="s" s="2">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="AO41" t="s" s="2">
         <v>84</v>
@@ -6793,10 +6791,10 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6819,16 +6817,16 @@
         <v>95</v>
       </c>
       <c r="K42" t="s" s="2">
+        <v>416</v>
+      </c>
+      <c r="L42" t="s" s="2">
         <v>417</v>
       </c>
-      <c r="L42" t="s" s="2">
+      <c r="M42" t="s" s="2">
         <v>418</v>
       </c>
-      <c r="M42" t="s" s="2">
+      <c r="N42" t="s" s="2">
         <v>419</v>
-      </c>
-      <c r="N42" t="s" s="2">
-        <v>420</v>
       </c>
       <c r="O42" s="2"/>
       <c r="P42" t="s" s="2">
@@ -6878,7 +6876,7 @@
         <v>84</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>82</v>
@@ -6899,10 +6897,10 @@
         <v>84</v>
       </c>
       <c r="AM42" t="s" s="2">
+        <v>420</v>
+      </c>
+      <c r="AN42" t="s" s="2">
         <v>421</v>
-      </c>
-      <c r="AN42" t="s" s="2">
-        <v>422</v>
       </c>
       <c r="AO42" t="s" s="2">
         <v>84</v>
@@ -6913,10 +6911,10 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -6939,16 +6937,16 @@
         <v>95</v>
       </c>
       <c r="K43" t="s" s="2">
+        <v>423</v>
+      </c>
+      <c r="L43" t="s" s="2">
         <v>424</v>
       </c>
-      <c r="L43" t="s" s="2">
+      <c r="M43" t="s" s="2">
         <v>425</v>
       </c>
-      <c r="M43" t="s" s="2">
+      <c r="N43" t="s" s="2">
         <v>426</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>427</v>
       </c>
       <c r="O43" s="2"/>
       <c r="P43" t="s" s="2">
@@ -6998,7 +6996,7 @@
         <v>84</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>82</v>
@@ -7019,10 +7017,10 @@
         <v>84</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AN43" t="s" s="2">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="AO43" t="s" s="2">
         <v>84</v>
@@ -7033,10 +7031,10 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -7059,19 +7057,19 @@
         <v>95</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="L44" t="s" s="2">
+        <v>429</v>
+      </c>
+      <c r="M44" t="s" s="2">
         <v>430</v>
       </c>
-      <c r="M44" t="s" s="2">
+      <c r="N44" t="s" s="2">
         <v>431</v>
       </c>
-      <c r="N44" t="s" s="2">
+      <c r="O44" t="s" s="2">
         <v>432</v>
-      </c>
-      <c r="O44" t="s" s="2">
-        <v>433</v>
       </c>
       <c r="P44" t="s" s="2">
         <v>84</v>
@@ -7120,7 +7118,7 @@
         <v>84</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>82</v>
@@ -7141,10 +7139,10 @@
         <v>84</v>
       </c>
       <c r="AM44" t="s" s="2">
+        <v>433</v>
+      </c>
+      <c r="AN44" t="s" s="2">
         <v>434</v>
-      </c>
-      <c r="AN44" t="s" s="2">
-        <v>435</v>
       </c>
       <c r="AO44" t="s" s="2">
         <v>84</v>
@@ -7155,10 +7153,10 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -7181,13 +7179,13 @@
         <v>84</v>
       </c>
       <c r="K45" t="s" s="2">
+        <v>365</v>
+      </c>
+      <c r="L45" t="s" s="2">
         <v>366</v>
       </c>
-      <c r="L45" t="s" s="2">
+      <c r="M45" t="s" s="2">
         <v>367</v>
-      </c>
-      <c r="M45" t="s" s="2">
-        <v>368</v>
       </c>
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
@@ -7238,7 +7236,7 @@
         <v>84</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>82</v>
@@ -7262,7 +7260,7 @@
         <v>84</v>
       </c>
       <c r="AN45" t="s" s="2">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="AO45" t="s" s="2">
         <v>84</v>
@@ -7273,10 +7271,10 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -7305,7 +7303,7 @@
         <v>141</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="N46" t="s" s="2">
         <v>143</v>
@@ -7358,7 +7356,7 @@
         <v>84</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>82</v>
@@ -7382,7 +7380,7 @@
         <v>84</v>
       </c>
       <c r="AN46" t="s" s="2">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="AO46" t="s" s="2">
         <v>84</v>
@@ -7393,14 +7391,14 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" t="s" s="2">
@@ -7422,10 +7420,10 @@
         <v>140</v>
       </c>
       <c r="L47" t="s" s="2">
+        <v>375</v>
+      </c>
+      <c r="M47" t="s" s="2">
         <v>376</v>
-      </c>
-      <c r="M47" t="s" s="2">
-        <v>377</v>
       </c>
       <c r="N47" t="s" s="2">
         <v>143</v>
@@ -7480,7 +7478,7 @@
         <v>84</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>82</v>
@@ -7515,10 +7513,10 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -7544,13 +7542,13 @@
         <v>192</v>
       </c>
       <c r="L48" t="s" s="2">
+        <v>439</v>
+      </c>
+      <c r="M48" t="s" s="2">
         <v>440</v>
       </c>
-      <c r="M48" t="s" s="2">
+      <c r="N48" t="s" s="2">
         <v>441</v>
-      </c>
-      <c r="N48" t="s" s="2">
-        <v>442</v>
       </c>
       <c r="O48" t="s" s="2">
         <v>211</v>
@@ -7578,13 +7576,13 @@
         <v>84</v>
       </c>
       <c r="X48" t="s" s="2">
-        <v>213</v>
+        <v>321</v>
       </c>
       <c r="Y48" t="s" s="2">
-        <v>214</v>
+        <v>442</v>
       </c>
       <c r="Z48" t="s" s="2">
-        <v>215</v>
+        <v>443</v>
       </c>
       <c r="AA48" t="s" s="2">
         <v>84</v>
@@ -7602,7 +7600,7 @@
         <v>84</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>94</v>
@@ -7620,16 +7618,16 @@
         <v>84</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="AM48" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="AN48" t="s" s="2">
         <v>218</v>
       </c>
-      <c r="AN48" t="s" s="2">
+      <c r="AO48" t="s" s="2">
         <v>219</v>
-      </c>
-      <c r="AO48" t="s" s="2">
-        <v>220</v>
       </c>
       <c r="AP48" t="s" s="2">
         <v>84</v>
@@ -7637,10 +7635,10 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -7663,19 +7661,19 @@
         <v>95</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="O49" t="s" s="2">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="P49" t="s" s="2">
         <v>84</v>
@@ -7724,7 +7722,7 @@
         <v>84</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>82</v>
@@ -7742,27 +7740,27 @@
         <v>84</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AM49" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="AN49" t="s" s="2">
+        <v>286</v>
+      </c>
+      <c r="AO49" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AP49" t="s" s="2">
         <v>287</v>
-      </c>
-      <c r="AN49" t="s" s="2">
-        <v>288</v>
-      </c>
-      <c r="AO49" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AP49" t="s" s="2">
-        <v>289</v>
       </c>
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
@@ -7788,16 +7786,16 @@
         <v>192</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="N50" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="O50" t="s" s="2">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="P50" t="s" s="2">
         <v>84</v>
@@ -7822,13 +7820,13 @@
         <v>84</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>282</v>
+        <v>212</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="Z50" t="s" s="2">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="AA50" t="s" s="2">
         <v>84</v>
@@ -7846,7 +7844,7 @@
         <v>84</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>82</v>
@@ -7855,7 +7853,7 @@
         <v>94</v>
       </c>
       <c r="AI50" t="s" s="2">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AJ50" t="s" s="2">
         <v>106</v>
@@ -7870,7 +7868,7 @@
         <v>137</v>
       </c>
       <c r="AN50" t="s" s="2">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AO50" t="s" s="2">
         <v>84</v>
@@ -7881,14 +7879,14 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" t="s" s="2">
@@ -7910,16 +7908,16 @@
         <v>192</v>
       </c>
       <c r="L51" t="s" s="2">
+        <v>299</v>
+      </c>
+      <c r="M51" t="s" s="2">
+        <v>300</v>
+      </c>
+      <c r="N51" t="s" s="2">
         <v>301</v>
       </c>
-      <c r="M51" t="s" s="2">
+      <c r="O51" t="s" s="2">
         <v>302</v>
-      </c>
-      <c r="N51" t="s" s="2">
-        <v>303</v>
-      </c>
-      <c r="O51" t="s" s="2">
-        <v>304</v>
       </c>
       <c r="P51" t="s" s="2">
         <v>84</v>
@@ -7944,13 +7942,13 @@
         <v>84</v>
       </c>
       <c r="X51" t="s" s="2">
-        <v>282</v>
+        <v>212</v>
       </c>
       <c r="Y51" t="s" s="2">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="Z51" t="s" s="2">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="AA51" t="s" s="2">
         <v>84</v>
@@ -7968,7 +7966,7 @@
         <v>84</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>82</v>
@@ -7986,27 +7984,27 @@
         <v>84</v>
       </c>
       <c r="AL51" t="s" s="2">
+        <v>305</v>
+      </c>
+      <c r="AM51" t="s" s="2">
+        <v>306</v>
+      </c>
+      <c r="AN51" t="s" s="2">
         <v>307</v>
       </c>
-      <c r="AM51" t="s" s="2">
+      <c r="AO51" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AP51" t="s" s="2">
         <v>308</v>
-      </c>
-      <c r="AN51" t="s" s="2">
-        <v>309</v>
-      </c>
-      <c r="AO51" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AP51" t="s" s="2">
-        <v>310</v>
       </c>
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -8032,16 +8030,16 @@
         <v>85</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="N52" t="s" s="2">
+        <v>359</v>
+      </c>
+      <c r="O52" t="s" s="2">
         <v>360</v>
-      </c>
-      <c r="O52" t="s" s="2">
-        <v>361</v>
       </c>
       <c r="P52" t="s" s="2">
         <v>84</v>
@@ -8090,7 +8088,7 @@
         <v>84</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>82</v>
@@ -8111,10 +8109,10 @@
         <v>84</v>
       </c>
       <c r="AM52" t="s" s="2">
+        <v>362</v>
+      </c>
+      <c r="AN52" t="s" s="2">
         <v>363</v>
-      </c>
-      <c r="AN52" t="s" s="2">
-        <v>364</v>
       </c>
       <c r="AO52" t="s" s="2">
         <v>84</v>

</xml_diff>